<commit_message>
IMC-621 fix bug in fcl_inserter
Former-commit-id: 6306d7d3ff3b221e997a25f6b980c68b2ff6a509
</commit_message>
<xml_diff>
--- a/app/classes/data_reader/__fakedata/schryver__FCL_fake_with_ranges.xlsx
+++ b/app/classes/data_reader/__fakedata/schryver__FCL_fake_with_ranges.xlsx
@@ -59,7 +59,7 @@
     <t xml:space="preserve">LOAD_TYPE</t>
   </si>
   <si>
-    <t xml:space="preserve">TYPE</t>
+    <t xml:space="preserve">RATE_BASIS</t>
   </si>
   <si>
     <t xml:space="preserve">TRANSIT_TIME</t>
@@ -422,7 +422,7 @@
     <tableColumn id="9" name="CARRIER"/>
     <tableColumn id="10" name="SERVICE_LEVEL"/>
     <tableColumn id="11" name="LOAD_TYPE"/>
-    <tableColumn id="12" name="TYPE"/>
+    <tableColumn id="12" name="RATE_BASIS"/>
     <tableColumn id="13" name="RANGE_MIN"/>
     <tableColumn id="14" name="RANGE_MAX"/>
     <tableColumn id="15" name="CURRENCY"/>
@@ -440,8 +440,8 @@
   </sheetPr>
   <dimension ref="A1:Z377"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A359" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B189"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M10" activeCellId="0" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23673,8 +23673,8 @@
   </sheetPr>
   <dimension ref="A1:R190"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A168" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B189"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M8" activeCellId="0" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>